<commit_message>
Update Wells coding manual_version4_anonymised.xlsx
Methods and materials including questionnaires, game and meeting scripts, observation sheets, data coding schemes, ethics applications
</commit_message>
<xml_diff>
--- a/Wells/Wells data coding scheme/Wells coding manual_version4_anonymised.xlsx
+++ b/Wells/Wells data coding scheme/Wells coding manual_version4_anonymised.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaktilamba/Dropbox/Everything/Github/demography-cooperation/Wells/Wells data coding scheme/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D86F045-7FDA-7F43-8632-7B9876D114FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C1A911-C9C6-074A-B609-E7CC148B110C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ethogram_version1" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -564,13 +563,13 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="29">
@@ -1379,226 +1378,226 @@
       <c r="J19" s="7"/>
     </row>
     <row r="20" spans="1:10" ht="30" customHeight="1">
-      <c r="A20" s="23" t="s">
+      <c r="A20" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
       <c r="J26" s="7"/>
     </row>
     <row r="27" spans="1:10" ht="43" customHeight="1">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
       <c r="J27" s="7"/>
     </row>
     <row r="28" spans="1:10" ht="22" customHeight="1">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
     </row>
     <row r="29" spans="1:10" ht="18" customHeight="1">
-      <c r="A29" s="23" t="s">
+      <c r="A29" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
     </row>
     <row r="30" spans="1:10" ht="25" customHeight="1">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="23"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
     </row>
     <row r="31" spans="1:10" ht="54" customHeight="1">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="23"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
     </row>
     <row r="32" spans="1:10" ht="28" customHeight="1">
-      <c r="A32" s="23" t="s">
+      <c r="A32" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="23"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
       <c r="I32" s="7"/>
       <c r="J32" s="7"/>
     </row>
     <row r="33" spans="1:10" ht="51" customHeight="1">
-      <c r="A33" s="23" t="s">
+      <c r="A33" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="23"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
     </row>
     <row r="34" spans="1:10" ht="22" customHeight="1">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="B34" s="23"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="23"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
     </row>
     <row r="35" spans="1:10" ht="57" customHeight="1">
-      <c r="A35" s="23" t="s">
+      <c r="A35" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="B35" s="23"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
     </row>
@@ -1645,48 +1644,48 @@
       <c r="J38" s="12"/>
     </row>
     <row r="39" spans="1:10" ht="32" customHeight="1">
-      <c r="A39" s="21" t="s">
+      <c r="A39" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
     </row>
     <row r="40" spans="1:10" ht="45" customHeight="1">
-      <c r="A40" s="21" t="s">
+      <c r="A40" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="B40" s="21"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="21"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23"/>
     </row>
     <row r="41" spans="1:10" ht="76" customHeight="1">
-      <c r="A41" s="21" t="s">
+      <c r="A41" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="B41" s="21"/>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="21"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="1:10" ht="73" customHeight="1">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="B42" s="21"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="21"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="23"/>
     </row>
     <row r="43" spans="1:10" ht="168" customHeight="1">
       <c r="A43" s="22" t="s">
@@ -1713,15 +1712,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A31:H31"/>
-    <mergeCell ref="A25:H25"/>
-    <mergeCell ref="A26:I26"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="A23:H23"/>
-    <mergeCell ref="A24:H24"/>
     <mergeCell ref="A44:G44"/>
     <mergeCell ref="A27:I27"/>
     <mergeCell ref="A28:J28"/>
@@ -1738,21 +1728,18 @@
     <mergeCell ref="A39:G39"/>
     <mergeCell ref="A40:G40"/>
     <mergeCell ref="A30:H30"/>
+    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="A26:I26"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="A24:H24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>